<commit_message>
byd, igt, deleted old unused
</commit_message>
<xml_diff>
--- a/Gaming/MLCO.xlsx
+++ b/Gaming/MLCO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\models\Gaming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE6B985-B6CF-4FBF-B872-6D23A0284BCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC27D89-6390-427D-864B-8AFD59688CE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -610,7 +610,7 @@
     <numFmt numFmtId="165" formatCode="0.000%"/>
     <numFmt numFmtId="166" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -676,12 +676,6 @@
       <color rgb="FF232A31"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="10">
@@ -834,7 +828,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -956,9 +950,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -14960,8 +14951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15550,10 +15541,10 @@
   <dimension ref="A1:X90"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H35" sqref="H35"/>
+      <selection pane="bottomRight" activeCell="C36" sqref="C36:F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16079,11 +16070,11 @@
         <f>F13+F14+F15</f>
         <v>-401.85800000000023</v>
       </c>
-      <c r="G16" s="83">
+      <c r="G16" s="11">
         <f>G13+G14+G15</f>
         <v>-400</v>
       </c>
-      <c r="H16" s="83">
+      <c r="H16" s="11">
         <f>H13+H14+H15</f>
         <v>-400</v>
       </c>
@@ -16588,10 +16579,10 @@
         <f>F19/F30</f>
         <v>1321.5904761904774</v>
       </c>
-      <c r="G29" s="84">
+      <c r="G29" s="10">
         <v>1322</v>
       </c>
-      <c r="H29" s="85">
+      <c r="H29" s="41">
         <v>1322</v>
       </c>
       <c r="K29" s="10"/>
@@ -17000,7 +16991,7 @@
       </c>
       <c r="B37" s="73"/>
       <c r="C37" s="57">
-        <f t="shared" ref="C37:H37" si="9">-C14/C13</f>
+        <f t="shared" ref="C37:F37" si="9">-C14/C13</f>
         <v>0</v>
       </c>
       <c r="D37" s="57">

</xml_diff>